<commit_message>
implemented the pagination for General and large taxcode monthly package
</commit_message>
<xml_diff>
--- a/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Suite GeneralAndLargeTaxcodeMonthly201718.xlsx
+++ b/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Suite GeneralAndLargeTaxcodeMonthly201718.xlsx
@@ -12,7 +12,7 @@
     <sheet name="ProcessPayrollForMonthlyTax" sheetId="4" r:id="rId3"/>
     <sheet name="TestReports" sheetId="5" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -642,7 +642,7 @@
     <col min="1" max="1" width="31" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="38.33203125" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="33.5546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.44140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -725,8 +725,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -786,7 +786,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
         <v>50</v>
       </c>

</xml_diff>